<commit_message>
finish fixes in add dash
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -454,10 +454,10 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>846814.23</v>
+        <v>994314.84</v>
       </c>
       <c r="C7">
-        <v>-80.9625674477055</v>
+        <v>-77.64657107587163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish refactor of add script
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,65 +399,54 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2">
-        <v>162593.82</v>
+        <v>950468.77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3">
-        <v>957144.34</v>
+        <v>1766113.68</v>
       </c>
       <c r="C3">
-        <v>488.6720294781191</v>
+        <v>85.81501420609537</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B4">
-        <v>1772367.68</v>
+        <v>2842827.64</v>
       </c>
       <c r="C4">
-        <v>85.17245580744905</v>
+        <v>60.96515599154411</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5">
-        <v>2845386.58</v>
+        <v>4442894.22</v>
       </c>
       <c r="C5">
-        <v>60.5415519651092</v>
+        <v>56.28433315781323</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B6">
-        <v>4448153.54</v>
+        <v>1014612.85</v>
       </c>
       <c r="C6">
-        <v>56.3286187987855</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>2025</v>
-      </c>
-      <c r="B7">
-        <v>994314.84</v>
-      </c>
-      <c r="C7">
-        <v>-77.64657107587163</v>
+        <v>-77.1632454035784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
terminei vendas BIBI e arrumei vendas ADD na analise e no dash
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ano</t>
   </si>
   <si>
-    <t>total_item</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Evolucao (%)</t>
+    <t>Evolução Total (%)</t>
+  </si>
+  <si>
+    <t>Qtd Produtos</t>
   </si>
 </sst>
 </file>
@@ -380,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,57 +399,89 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>23866.41</v>
+      </c>
+      <c r="D2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>2021</v>
       </c>
-      <c r="B2">
-        <v>950468.77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="B3">
+        <v>279918.14</v>
+      </c>
+      <c r="C3">
+        <v>1072.853981809581</v>
+      </c>
+      <c r="D3">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>2022</v>
       </c>
-      <c r="B3">
-        <v>1766113.68</v>
-      </c>
-      <c r="C3">
-        <v>85.81501420609537</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="B4">
+        <v>504349.28</v>
+      </c>
+      <c r="C4">
+        <v>80.17741901257274</v>
+      </c>
+      <c r="D4">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>2023</v>
       </c>
-      <c r="B4">
-        <v>2842827.64</v>
-      </c>
-      <c r="C4">
-        <v>60.96515599154411</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="B5">
+        <v>802464.89</v>
+      </c>
+      <c r="C5">
+        <v>59.1089591721039</v>
+      </c>
+      <c r="D5">
+        <v>3337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>2024</v>
       </c>
-      <c r="B5">
-        <v>4442894.22</v>
-      </c>
-      <c r="C5">
-        <v>56.28433315781323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="B6">
+        <v>1197062.47</v>
+      </c>
+      <c r="C6">
+        <v>49.17318937156241</v>
+      </c>
+      <c r="D6">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>2025</v>
       </c>
-      <c r="B6">
-        <v>1014612.85</v>
-      </c>
-      <c r="C6">
-        <v>-77.1632454035784</v>
+      <c r="B7">
+        <v>396607.32</v>
+      </c>
+      <c r="C7">
+        <v>-66.86828549557652</v>
+      </c>
+      <c r="D7">
+        <v>1635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizei dados para BIBI e ADD 06-05-2025
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -475,13 +475,13 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>396607.32</v>
+        <v>421672.91</v>
       </c>
       <c r="C7">
-        <v>-66.86828549557652</v>
+        <v>-64.77436052272193</v>
       </c>
       <c r="D7">
-        <v>1635</v>
+        <v>1729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizei dados da add de faturamento
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -408,7 +408,7 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>23866.41</v>
+        <v>116037.66</v>
       </c>
       <c r="D2">
         <v>262</v>
@@ -419,10 +419,10 @@
         <v>2021</v>
       </c>
       <c r="B3">
-        <v>279918.14</v>
+        <v>956806.1899999999</v>
       </c>
       <c r="C3">
-        <v>1072.853981809581</v>
+        <v>724.5652230491376</v>
       </c>
       <c r="D3">
         <v>2168</v>
@@ -433,10 +433,10 @@
         <v>2022</v>
       </c>
       <c r="B4">
-        <v>504349.28</v>
+        <v>1772410.88</v>
       </c>
       <c r="C4">
-        <v>80.17741901257274</v>
+        <v>85.24241361774634</v>
       </c>
       <c r="D4">
         <v>2708</v>
@@ -447,10 +447,10 @@
         <v>2023</v>
       </c>
       <c r="B5">
-        <v>802464.89</v>
+        <v>2846150.66</v>
       </c>
       <c r="C5">
-        <v>59.1089591721039</v>
+        <v>60.58074863544059</v>
       </c>
       <c r="D5">
         <v>3337</v>
@@ -461,10 +461,10 @@
         <v>2024</v>
       </c>
       <c r="B6">
-        <v>1197062.47</v>
+        <v>4457482.68</v>
       </c>
       <c r="C6">
-        <v>49.17318937156241</v>
+        <v>56.61443164783131</v>
       </c>
       <c r="D6">
         <v>4742</v>
@@ -475,13 +475,13 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>421672.91</v>
+        <v>1989051.38</v>
       </c>
       <c r="C7">
-        <v>-64.77436052272193</v>
+        <v>-55.3772493850722</v>
       </c>
       <c r="D7">
-        <v>1729</v>
+        <v>1746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alterei modelagem de rfma recorrencia retencao e faturamentos da add para banco padrao e carreguei dados novos para add e bibi
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -408,10 +408,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>116037.66</v>
+        <v>115677.51</v>
       </c>
       <c r="D2">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -419,13 +419,13 @@
         <v>2021</v>
       </c>
       <c r="B3">
-        <v>956806.1899999999</v>
+        <v>953108.38</v>
       </c>
       <c r="C3">
-        <v>724.5652230491376</v>
+        <v>723.9357676353857</v>
       </c>
       <c r="D3">
-        <v>2168</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -433,13 +433,13 @@
         <v>2022</v>
       </c>
       <c r="B4">
-        <v>1772410.88</v>
+        <v>1786705.19</v>
       </c>
       <c r="C4">
-        <v>85.24241361774634</v>
+        <v>87.46086253065994</v>
       </c>
       <c r="D4">
-        <v>2708</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -447,13 +447,13 @@
         <v>2023</v>
       </c>
       <c r="B5">
-        <v>2846150.66</v>
+        <v>2885974.02</v>
       </c>
       <c r="C5">
-        <v>60.58074863544059</v>
+        <v>61.52491391151107</v>
       </c>
       <c r="D5">
-        <v>3337</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -461,13 +461,13 @@
         <v>2024</v>
       </c>
       <c r="B6">
-        <v>4457482.68</v>
+        <v>4517432.77</v>
       </c>
       <c r="C6">
-        <v>56.61443164783131</v>
+        <v>56.53061111062945</v>
       </c>
       <c r="D6">
-        <v>4742</v>
+        <v>4662</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -475,13 +475,13 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>1989051.38</v>
+        <v>1774017.75</v>
       </c>
       <c r="C7">
-        <v>-55.3772493850722</v>
+        <v>-60.72951518435104</v>
       </c>
       <c r="D7">
-        <v>1746</v>
+        <v>1680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao de dados da add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -475,13 +475,13 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>1774017.75</v>
+        <v>1910102.1</v>
       </c>
       <c r="C7">
-        <v>-60.72951518435104</v>
+        <v>-57.71708850467297</v>
       </c>
       <c r="D7">
-        <v>1680</v>
+        <v>1823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao de dados e mudanca da tela principal
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -475,13 +475,13 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>1910102.1</v>
+        <v>1959641.72</v>
       </c>
       <c r="C7">
-        <v>-57.71708850467297</v>
+        <v>-56.62045635711807</v>
       </c>
       <c r="D7">
-        <v>1823</v>
+        <v>1868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcao no dash e nas modelagens de transacao
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ano</t>
   </si>
@@ -26,6 +26,15 @@
   </si>
   <si>
     <t>Qtd Produtos</t>
+  </si>
+  <si>
+    <t>Qtd Vendas</t>
+  </si>
+  <si>
+    <t>Ticket Médio Anual</t>
+  </si>
+  <si>
+    <t>Evolução Ticket Médio (%)</t>
   </si>
 </sst>
 </file>
@@ -383,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +411,17 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -413,8 +431,14 @@
       <c r="D2">
         <v>258</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>258</v>
+      </c>
+      <c r="F2">
+        <v>448.3624418604651</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -427,8 +451,17 @@
       <c r="D3">
         <v>2141</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>2141</v>
+      </c>
+      <c r="F3">
+        <v>445.1697244278375</v>
+      </c>
+      <c r="G3">
+        <v>-0.712084049542494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -441,8 +474,17 @@
       <c r="D4">
         <v>2716</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>2716</v>
+      </c>
+      <c r="F4">
+        <v>657.8443262150221</v>
+      </c>
+      <c r="G4">
+        <v>47.77382425557543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -455,8 +497,17 @@
       <c r="D5">
         <v>3342</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>3342</v>
+      </c>
+      <c r="F5">
+        <v>863.5469838420108</v>
+      </c>
+      <c r="G5">
+        <v>31.26919993526753</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -469,8 +520,17 @@
       <c r="D6">
         <v>4662</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>4662</v>
+      </c>
+      <c r="F6">
+        <v>968.9902981552981</v>
+      </c>
+      <c r="G6">
+        <v>12.21048956064428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -482,6 +542,15 @@
       </c>
       <c r="D7">
         <v>1887</v>
+      </c>
+      <c r="E7">
+        <v>1887</v>
+      </c>
+      <c r="F7">
+        <v>1046.919337572867</v>
+      </c>
+      <c r="G7">
+        <v>8.04229305142945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao dos dados bibi add e bdxp
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/faturamento_anual.xlsx
@@ -535,22 +535,22 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>2002837.36</v>
+        <v>2038323.67</v>
       </c>
       <c r="C7">
-        <v>-55.66425751146264</v>
+        <v>-54.87871599249057</v>
       </c>
       <c r="D7">
-        <v>1922</v>
+        <v>1951</v>
       </c>
       <c r="E7">
-        <v>1922</v>
+        <v>1951</v>
       </c>
       <c r="F7">
-        <v>1042.058980228928</v>
+        <v>1044.758416196822</v>
       </c>
       <c r="G7">
-        <v>7.54070316418376</v>
+        <v>7.819285516662711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>